<commit_message>
going over first chapter in quick-start
</commit_message>
<xml_diff>
--- a/R/quick-start/MyResults.xlsx
+++ b/R/quick-start/MyResults.xlsx
@@ -22,7 +22,7 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Dec/13/2022</t>
+    <t xml:space="preserve">Apr/23/2023</t>
   </si>
   <si>
     <t xml:space="preserve">Output file</t>
@@ -918,7 +918,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.0108548168249661</v>
+        <v>0.010854816824966</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1037,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.0000233199415316389</v>
+        <v>0.000023319941531639</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1046,7 +1046,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>-0.000683891460998864</v>
+        <v>-0.000683891460998863</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -1058,7 +1058,7 @@
         <v>0.000791682146950474</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>0.518871720080713</v>
+        <v>0.518871720080714</v>
       </c>
     </row>
     <row r="12">
@@ -1069,7 +1069,7 @@
         <v>0.000483637672681172</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>0.316978110579537</v>
+        <v>0.316978110579538</v>
       </c>
     </row>
     <row r="13">
@@ -1088,7 +1088,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.00152577624933447</v>
+        <v>0.00152577624933446</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -1111,7 +1111,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.0000233199415316389</v>
+        <v>0.000023319941531639</v>
       </c>
     </row>
     <row r="19">
@@ -1127,7 +1127,7 @@
         <v>49</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>-0.000683891460998864</v>
+        <v>-0.000683891460998863</v>
       </c>
     </row>
     <row r="21">
@@ -1135,7 +1135,7 @@
         <v>56</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>-0.00288714747448691</v>
+        <v>-0.00288714747448689</v>
       </c>
     </row>
     <row r="22">
@@ -1151,7 +1151,7 @@
         <v>58</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.0762965577128861</v>
+        <v>0.076296557712886</v>
       </c>
     </row>
     <row r="25">
@@ -1271,7 +1271,7 @@
         <v>0.00151860581999368</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>0.000715813263459218</v>
+        <v>0.000715813263459217</v>
       </c>
     </row>
     <row r="34">
@@ -1285,10 +1285,10 @@
         <v>0.000147692932074957</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>0.00137737876647313</v>
+        <v>0.00137737876647312</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>0.000765088967603179</v>
+        <v>0.00076508896760318</v>
       </c>
     </row>
     <row r="35">
@@ -1438,7 +1438,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.0108548168249661</v>
+        <v>0.010854816824966</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.00501012182412403</v>
@@ -1447,16 +1447,16 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>2.16657742187018</v>
+        <v>2.16657742187016</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.118837857481057</v>
+        <v>0.118837857481059</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>-0.00508962686323864</v>
+        <v>-0.00508962686323875</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>0.0267992605131709</v>
+        <v>0.0267992605131708</v>
       </c>
     </row>
     <row r="10">
@@ -1602,7 +1602,7 @@
         <v>0.000235654096607136</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.321013472035591</v>
+        <v>0.321013472035592</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -1616,7 +1616,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.000734094102383992</v>
+        <v>0.000734094102383991</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1661,22 +1661,22 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.0108548168249661</v>
+        <v>0.010854816824966</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.0191584720474258</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.566580507991222</v>
+        <v>0.566580507991217</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0.570999221045945</v>
+        <v>0.570999221045949</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>-0.0266950983868058</v>
+        <v>-0.0266950983868059</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>0.0484047320367381</v>
+        <v>0.0484047320367379</v>
       </c>
     </row>
     <row r="10">
@@ -1800,10 +1800,10 @@
         <v>0.928415092542449</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>-0.0800268093513029</v>
+        <v>-0.0800268093513028</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>0.087715637935654</v>
+        <v>0.0877156379356539</v>
       </c>
     </row>
     <row r="18">
@@ -1823,7 +1823,7 @@
         <v>0.59185327361744</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>-0.0570517813022475</v>
+        <v>-0.0570517813022476</v>
       </c>
       <c r="G18" s="1" t="n">
         <v>0.100018764567738</v>
@@ -1837,19 +1837,19 @@
         <v>0.0171867933061963</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>0.0349939937380673</v>
+        <v>0.0349939937380672</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>0.491135519850657</v>
+        <v>0.491135519850658</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>0.623330600567419</v>
+        <v>0.623330600567418</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>-0.0514001740956357</v>
+        <v>-0.0514001740956356</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>0.0857737607080284</v>
+        <v>0.0857737607080283</v>
       </c>
     </row>
     <row r="20">
@@ -1863,16 +1863,16 @@
         <v>0.0348053648276017</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>0.0259893287493949</v>
+        <v>0.025989328749395</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>0.979265850001879</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>-0.0673126934621294</v>
+        <v>-0.0673126934621293</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>0.0691218295996237</v>
+        <v>0.0691218295996236</v>
       </c>
     </row>
   </sheetData>
@@ -2004,7 +2004,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.0108548168249661</v>
+        <v>0.010854816824966</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.00501012182412403</v>
@@ -2013,16 +2013,16 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>2.16657742187018</v>
+        <v>2.16657742187016</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.118837857481057</v>
+        <v>0.118837857481059</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>-0.00508962686323864</v>
+        <v>-0.00508962686323875</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>0.0267992605131709</v>
+        <v>0.0267992605131708</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
after fixing Rjafroc Ss RSM NH model
</commit_message>
<xml_diff>
--- a/R/quick-start/MyResults.xlsx
+++ b/R/quick-start/MyResults.xlsx
@@ -22,7 +22,7 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Apr/23/2023</t>
+    <t xml:space="preserve">May/07/2023</t>
   </si>
   <si>
     <t xml:space="preserve">Output file</t>
@@ -918,7 +918,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.010854816824966</v>
+        <v>0.0108548168249661</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1037,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.000023319941531639</v>
+        <v>0.0000233199415316389</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1046,7 +1046,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>-0.000683891460998863</v>
+        <v>-0.000683891460998864</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -1058,7 +1058,7 @@
         <v>0.000791682146950474</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>0.518871720080714</v>
+        <v>0.518871720080713</v>
       </c>
     </row>
     <row r="12">
@@ -1069,7 +1069,7 @@
         <v>0.000483637672681172</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>0.316978110579538</v>
+        <v>0.316978110579537</v>
       </c>
     </row>
     <row r="13">
@@ -1088,7 +1088,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.00152577624933446</v>
+        <v>0.00152577624933447</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -1111,7 +1111,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.000023319941531639</v>
+        <v>0.0000233199415316389</v>
       </c>
     </row>
     <row r="19">
@@ -1127,7 +1127,7 @@
         <v>49</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>-0.000683891460998863</v>
+        <v>-0.000683891460998864</v>
       </c>
     </row>
     <row r="21">
@@ -1135,7 +1135,7 @@
         <v>56</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>-0.00288714747448689</v>
+        <v>-0.00288714747448691</v>
       </c>
     </row>
     <row r="22">
@@ -1151,7 +1151,7 @@
         <v>58</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.076296557712886</v>
+        <v>0.0762965577128861</v>
       </c>
     </row>
     <row r="25">
@@ -1271,7 +1271,7 @@
         <v>0.00151860581999368</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>0.000715813263459217</v>
+        <v>0.000715813263459218</v>
       </c>
     </row>
     <row r="34">
@@ -1285,10 +1285,10 @@
         <v>0.000147692932074957</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>0.00137737876647312</v>
+        <v>0.00137737876647313</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>0.00076508896760318</v>
+        <v>0.000765088967603179</v>
       </c>
     </row>
     <row r="35">
@@ -1438,7 +1438,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.010854816824966</v>
+        <v>0.0108548168249661</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.00501012182412403</v>
@@ -1447,16 +1447,16 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>2.16657742187016</v>
+        <v>2.16657742187018</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.118837857481059</v>
+        <v>0.118837857481057</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>-0.00508962686323875</v>
+        <v>-0.00508962686323864</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>0.0267992605131708</v>
+        <v>0.0267992605131709</v>
       </c>
     </row>
     <row r="10">
@@ -1602,7 +1602,7 @@
         <v>0.000235654096607136</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.321013472035592</v>
+        <v>0.321013472035591</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -1616,7 +1616,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.000734094102383991</v>
+        <v>0.000734094102383992</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1661,22 +1661,22 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.010854816824966</v>
+        <v>0.0108548168249661</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.0191584720474258</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.566580507991217</v>
+        <v>0.566580507991222</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0.570999221045949</v>
+        <v>0.570999221045945</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>-0.0266950983868059</v>
+        <v>-0.0266950983868058</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>0.0484047320367379</v>
+        <v>0.0484047320367381</v>
       </c>
     </row>
     <row r="10">
@@ -1800,10 +1800,10 @@
         <v>0.928415092542449</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>-0.0800268093513028</v>
+        <v>-0.0800268093513029</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>0.0877156379356539</v>
+        <v>0.087715637935654</v>
       </c>
     </row>
     <row r="18">
@@ -1823,7 +1823,7 @@
         <v>0.59185327361744</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>-0.0570517813022476</v>
+        <v>-0.0570517813022475</v>
       </c>
       <c r="G18" s="1" t="n">
         <v>0.100018764567738</v>
@@ -1837,19 +1837,19 @@
         <v>0.0171867933061963</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>0.0349939937380672</v>
+        <v>0.0349939937380673</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>0.491135519850658</v>
+        <v>0.491135519850657</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>0.623330600567418</v>
+        <v>0.623330600567419</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>-0.0514001740956356</v>
+        <v>-0.0514001740956357</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>0.0857737607080283</v>
+        <v>0.0857737607080284</v>
       </c>
     </row>
     <row r="20">
@@ -1863,16 +1863,16 @@
         <v>0.0348053648276017</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>0.025989328749395</v>
+        <v>0.0259893287493949</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>0.979265850001879</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>-0.0673126934621293</v>
+        <v>-0.0673126934621294</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>0.0691218295996236</v>
+        <v>0.0691218295996237</v>
       </c>
     </row>
   </sheetData>
@@ -2004,7 +2004,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.010854816824966</v>
+        <v>0.0108548168249661</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.00501012182412403</v>
@@ -2013,16 +2013,16 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>2.16657742187016</v>
+        <v>2.16657742187018</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.118837857481059</v>
+        <v>0.118837857481057</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>-0.00508962686323875</v>
+        <v>-0.00508962686323864</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>0.0267992605131708</v>
+        <v>0.0267992605131709</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
19- after moving SsFrocSampleSize code to RJafroc
</commit_message>
<xml_diff>
--- a/R/quick-start/MyResults.xlsx
+++ b/R/quick-start/MyResults.xlsx
@@ -22,7 +22,7 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">May/07/2023</t>
+    <t xml:space="preserve">May/08/2023</t>
   </si>
   <si>
     <t xml:space="preserve">Output file</t>
@@ -918,7 +918,7 @@
         <v>37</v>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.0108548168249661</v>
+        <v>0.010854816824966</v>
       </c>
     </row>
   </sheetData>
@@ -1037,7 +1037,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.0000233199415316389</v>
+        <v>0.000023319941531639</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1046,7 +1046,7 @@
         <v>49</v>
       </c>
       <c r="B10" s="1" t="n">
-        <v>-0.000683891460998864</v>
+        <v>-0.000683891460998863</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -1058,7 +1058,7 @@
         <v>0.000791682146950474</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>0.518871720080713</v>
+        <v>0.518871720080714</v>
       </c>
     </row>
     <row r="12">
@@ -1069,7 +1069,7 @@
         <v>0.000483637672681172</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>0.316978110579537</v>
+        <v>0.316978110579538</v>
       </c>
     </row>
     <row r="13">
@@ -1088,7 +1088,7 @@
         <v>53</v>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.00152577624933447</v>
+        <v>0.00152577624933446</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -1111,7 +1111,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.0000233199415316389</v>
+        <v>0.000023319941531639</v>
       </c>
     </row>
     <row r="19">
@@ -1127,7 +1127,7 @@
         <v>49</v>
       </c>
       <c r="B20" s="1" t="n">
-        <v>-0.000683891460998864</v>
+        <v>-0.000683891460998863</v>
       </c>
     </row>
     <row r="21">
@@ -1135,7 +1135,7 @@
         <v>56</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>-0.00288714747448691</v>
+        <v>-0.00288714747448689</v>
       </c>
     </row>
     <row r="22">
@@ -1151,7 +1151,7 @@
         <v>58</v>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.0762965577128861</v>
+        <v>0.076296557712886</v>
       </c>
     </row>
     <row r="25">
@@ -1271,7 +1271,7 @@
         <v>0.00151860581999368</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>0.000715813263459218</v>
+        <v>0.000715813263459217</v>
       </c>
     </row>
     <row r="34">
@@ -1285,10 +1285,10 @@
         <v>0.000147692932074957</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>0.00137737876647313</v>
+        <v>0.00137737876647312</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>0.000765088967603179</v>
+        <v>0.00076508896760318</v>
       </c>
     </row>
     <row r="35">
@@ -1438,7 +1438,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.0108548168249661</v>
+        <v>0.010854816824966</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.00501012182412403</v>
@@ -1447,16 +1447,16 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>2.16657742187018</v>
+        <v>2.16657742187016</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.118837857481057</v>
+        <v>0.118837857481059</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>-0.00508962686323864</v>
+        <v>-0.00508962686323875</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>0.0267992605131709</v>
+        <v>0.0267992605131708</v>
       </c>
     </row>
     <row r="10">
@@ -1602,7 +1602,7 @@
         <v>0.000235654096607136</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.321013472035591</v>
+        <v>0.321013472035592</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>1</v>
@@ -1616,7 +1616,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.000734094102383992</v>
+        <v>0.000734094102383991</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1661,22 +1661,22 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.0108548168249661</v>
+        <v>0.010854816824966</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.0191584720474258</v>
       </c>
       <c r="D8" s="1" t="n">
-        <v>0.566580507991222</v>
+        <v>0.566580507991217</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>0.570999221045945</v>
+        <v>0.570999221045949</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>-0.0266950983868058</v>
+        <v>-0.0266950983868059</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>0.0484047320367381</v>
+        <v>0.0484047320367379</v>
       </c>
     </row>
     <row r="10">
@@ -1800,10 +1800,10 @@
         <v>0.928415092542449</v>
       </c>
       <c r="F17" s="1" t="n">
-        <v>-0.0800268093513029</v>
+        <v>-0.0800268093513028</v>
       </c>
       <c r="G17" s="1" t="n">
-        <v>0.087715637935654</v>
+        <v>0.0877156379356539</v>
       </c>
     </row>
     <row r="18">
@@ -1823,7 +1823,7 @@
         <v>0.59185327361744</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>-0.0570517813022475</v>
+        <v>-0.0570517813022476</v>
       </c>
       <c r="G18" s="1" t="n">
         <v>0.100018764567738</v>
@@ -1837,19 +1837,19 @@
         <v>0.0171867933061963</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>0.0349939937380673</v>
+        <v>0.0349939937380672</v>
       </c>
       <c r="D19" s="1" t="n">
-        <v>0.491135519850657</v>
+        <v>0.491135519850658</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>0.623330600567419</v>
+        <v>0.623330600567418</v>
       </c>
       <c r="F19" s="1" t="n">
-        <v>-0.0514001740956357</v>
+        <v>-0.0514001740956356</v>
       </c>
       <c r="G19" s="1" t="n">
-        <v>0.0857737607080284</v>
+        <v>0.0857737607080283</v>
       </c>
     </row>
     <row r="20">
@@ -1863,16 +1863,16 @@
         <v>0.0348053648276017</v>
       </c>
       <c r="D20" s="1" t="n">
-        <v>0.0259893287493949</v>
+        <v>0.025989328749395</v>
       </c>
       <c r="E20" s="1" t="n">
         <v>0.979265850001879</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>-0.0673126934621294</v>
+        <v>-0.0673126934621293</v>
       </c>
       <c r="G20" s="1" t="n">
-        <v>0.0691218295996237</v>
+        <v>0.0691218295996236</v>
       </c>
     </row>
   </sheetData>
@@ -2004,7 +2004,7 @@
         <v>37</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.0108548168249661</v>
+        <v>0.010854816824966</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>0.00501012182412403</v>
@@ -2013,16 +2013,16 @@
         <v>3</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>2.16657742187018</v>
+        <v>2.16657742187016</v>
       </c>
       <c r="F8" s="1" t="n">
-        <v>0.118837857481057</v>
+        <v>0.118837857481059</v>
       </c>
       <c r="G8" s="1" t="n">
-        <v>-0.00508962686323864</v>
+        <v>-0.00508962686323875</v>
       </c>
       <c r="H8" s="1" t="n">
-        <v>0.0267992605131709</v>
+        <v>0.0267992605131708</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
wrapping up sample size; almost there
</commit_message>
<xml_diff>
--- a/R/quick-start/MyResults.xlsx
+++ b/R/quick-start/MyResults.xlsx
@@ -22,7 +22,7 @@
     <t xml:space="preserve">Date</t>
   </si>
   <si>
-    <t xml:space="preserve">May/08/2023</t>
+    <t xml:space="preserve">May/21/2023</t>
   </si>
   <si>
     <t xml:space="preserve">Output file</t>
@@ -1037,7 +1037,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.000023319941531639</v>
+        <v>0.0000233199415316389</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1111,7 +1111,7 @@
         <v>48</v>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.000023319941531639</v>
+        <v>0.0000233199415316389</v>
       </c>
     </row>
     <row r="19">
@@ -1135,7 +1135,7 @@
         <v>56</v>
       </c>
       <c r="B21" s="1" t="n">
-        <v>-0.00288714747448689</v>
+        <v>-0.00288714747448687</v>
       </c>
     </row>
     <row r="22">
@@ -1823,7 +1823,7 @@
         <v>0.59185327361744</v>
       </c>
       <c r="F18" s="1" t="n">
-        <v>-0.0570517813022476</v>
+        <v>-0.0570517813022475</v>
       </c>
       <c r="G18" s="1" t="n">
         <v>0.100018764567738</v>
@@ -1869,7 +1869,7 @@
         <v>0.979265850001879</v>
       </c>
       <c r="F20" s="1" t="n">
-        <v>-0.0673126934621293</v>
+        <v>-0.0673126934621292</v>
       </c>
       <c r="G20" s="1" t="n">
         <v>0.0691218295996236</v>

</xml_diff>